<commit_message>
Look at this GRAPH
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Clay/Clay 02-12-2024.xlsx
+++ b/P3/Results/Data/Clay/Clay 02-12-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mads\OneDrive\Dokumenter\GitHub\Robotteknologi-3.-semester\P3\Results\Data\Clay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED25A30-5729-4B98-8A03-02FC5FB2F6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6888108-8242-4F5B-981B-048257167D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4966,7 +4966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898C2D57-096F-442D-846A-938D525EB3D5}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>

</xml_diff>